<commit_message>
ECEN405 lab 2 report complete
</commit_message>
<xml_diff>
--- a/Tri 2/ECEN405/Lab 2/ECEN405 lab 2.xlsx
+++ b/Tri 2/ECEN405/Lab 2/ECEN405 lab 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\state-opera.ecs.vuw.ac.nz\claytoniel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niels\Desktop\Uni-Notes\Tri 2\ECEN405\Lab 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCCA37FE-D394-41D2-B5CD-C8C0ADE21CE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50567B8-9837-4049-8B34-74F95CE4502C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{471539E5-F71B-43F2-AC2A-5EA13CA541A5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21390" xr2:uid="{471539E5-F71B-43F2-AC2A-5EA13CA541A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -594,13 +603,27 @@
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  </a:sysClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -608,8 +631,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-NZ" b="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Efficiency</a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Effeciency vs Output Current</a:t>
+              <a:t> vs Output Current</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -626,13 +655,27 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:schemeClr>
+                </a:sysClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -882,6 +925,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ" sz="1600"/>
+                  <a:t>Output Current (mA)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -946,6 +1044,64 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Efficiency</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-NZ" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2190,15 +2346,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>14287</xdr:colOff>
+      <xdr:colOff>14286</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2526,7 +2682,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="AG42" sqref="AG28:AG42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2582,11 +2738,11 @@
         <v>1.4339999999999999E-2</v>
       </c>
       <c r="H2">
-        <f>POWER(F2,2)/100</f>
+        <f t="shared" ref="H2:H24" si="0">POWER(F2,2)/100</f>
         <v>2.0563559999999995E-2</v>
       </c>
       <c r="J2">
-        <f>(H2/D2)*100</f>
+        <f t="shared" ref="J2:J24" si="1">(H2/D2)*100</f>
         <v>50.774222222222207</v>
       </c>
       <c r="L2">
@@ -2605,22 +2761,22 @@
         <v>1.66E-3</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D6" si="0">C3*30</f>
+        <f t="shared" ref="D3:D6" si="2">C3*30</f>
         <v>4.9799999999999997E-2</v>
       </c>
       <c r="F3">
         <v>1.714</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G24" si="1">F3/100</f>
+        <f t="shared" ref="G3:G24" si="3">F3/100</f>
         <v>1.7139999999999999E-2</v>
       </c>
       <c r="H3">
-        <f>POWER(F3,2)/100</f>
+        <f t="shared" si="0"/>
         <v>2.9377960000000002E-2</v>
       </c>
       <c r="J3">
-        <f>(H3/D3)*100</f>
+        <f t="shared" si="1"/>
         <v>58.991887550200808</v>
       </c>
     </row>
@@ -2632,22 +2788,22 @@
         <v>2.0300000000000001E-3</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.0900000000000003E-2</v>
       </c>
       <c r="F4">
         <v>1.992</v>
       </c>
       <c r="G4">
+        <f t="shared" si="3"/>
+        <v>1.992E-2</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>3.9680640000000003E-2</v>
+      </c>
+      <c r="J4">
         <f t="shared" si="1"/>
-        <v>1.992E-2</v>
-      </c>
-      <c r="H4">
-        <f>POWER(F4,2)/100</f>
-        <v>3.9680640000000003E-2</v>
-      </c>
-      <c r="J4">
-        <f>(H4/D4)*100</f>
         <v>65.157044334975367</v>
       </c>
     </row>
@@ -2659,22 +2815,22 @@
         <v>2.4599999999999999E-3</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.3800000000000004E-2</v>
       </c>
       <c r="F5">
         <v>2.2679999999999998</v>
       </c>
       <c r="G5">
+        <f t="shared" si="3"/>
+        <v>2.2679999999999999E-2</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>5.1438239999999996E-2</v>
+      </c>
+      <c r="J5">
         <f t="shared" si="1"/>
-        <v>2.2679999999999999E-2</v>
-      </c>
-      <c r="H5">
-        <f>POWER(F5,2)/100</f>
-        <v>5.1438239999999996E-2</v>
-      </c>
-      <c r="J5">
-        <f>(H5/D5)*100</f>
         <v>69.69951219512194</v>
       </c>
     </row>
@@ -2686,22 +2842,22 @@
         <v>2.96E-3</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.8800000000000004E-2</v>
       </c>
       <c r="F6">
         <v>2.5419999999999998</v>
       </c>
       <c r="G6">
+        <f t="shared" si="3"/>
+        <v>2.5419999999999998E-2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>6.461763999999999E-2</v>
+      </c>
+      <c r="J6">
         <f t="shared" si="1"/>
-        <v>2.5419999999999998E-2</v>
-      </c>
-      <c r="H6">
-        <f>POWER(F6,2)/100</f>
-        <v>6.461763999999999E-2</v>
-      </c>
-      <c r="J6">
-        <f>(H6/D6)*100</f>
         <v>72.767612612612595</v>
       </c>
     </row>
@@ -2720,15 +2876,15 @@
         <v>2.8180000000000001</v>
       </c>
       <c r="G7">
+        <f t="shared" si="3"/>
+        <v>2.818E-2</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>7.9411240000000008E-2</v>
+      </c>
+      <c r="J7">
         <f t="shared" si="1"/>
-        <v>2.818E-2</v>
-      </c>
-      <c r="H7">
-        <f>POWER(F7,2)/100</f>
-        <v>7.9411240000000008E-2</v>
-      </c>
-      <c r="J7">
-        <f>(H7/D7)*100</f>
         <v>75.200037878787882</v>
       </c>
     </row>
@@ -2740,22 +2896,22 @@
         <v>7.1900000000000002E-3</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" ref="D8:D24" si="2">C8*30</f>
+        <f t="shared" ref="D8:D24" si="4">C8*30</f>
         <v>0.2157</v>
       </c>
       <c r="F8">
         <v>4.2030000000000003</v>
       </c>
       <c r="G8">
+        <f t="shared" si="3"/>
+        <v>4.2030000000000005E-2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0.17665209000000001</v>
+      </c>
+      <c r="J8">
         <f t="shared" si="1"/>
-        <v>4.2030000000000005E-2</v>
-      </c>
-      <c r="H8">
-        <f>POWER(F8,2)/100</f>
-        <v>0.17665209000000001</v>
-      </c>
-      <c r="J8">
-        <f>(H8/D8)*100</f>
         <v>81.897121001390829</v>
       </c>
     </row>
@@ -2767,22 +2923,22 @@
         <v>1.2319999999999999E-2</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.36959999999999998</v>
       </c>
       <c r="F9">
         <v>5.61</v>
       </c>
       <c r="G9">
+        <f t="shared" si="3"/>
+        <v>5.6100000000000004E-2</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>0.31472100000000003</v>
+      </c>
+      <c r="J9">
         <f t="shared" si="1"/>
-        <v>5.6100000000000004E-2</v>
-      </c>
-      <c r="H9">
-        <f>POWER(F9,2)/100</f>
-        <v>0.31472100000000003</v>
-      </c>
-      <c r="J9">
-        <f>(H9/D9)*100</f>
         <v>85.151785714285722</v>
       </c>
     </row>
@@ -2794,22 +2950,22 @@
         <v>1.891E-2</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.56730000000000003</v>
       </c>
       <c r="F10">
         <v>7.0289999999999999</v>
       </c>
       <c r="G10">
+        <f t="shared" si="3"/>
+        <v>7.0290000000000005E-2</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0.49406841000000001</v>
+      </c>
+      <c r="J10">
         <f t="shared" si="1"/>
-        <v>7.0290000000000005E-2</v>
-      </c>
-      <c r="H10">
-        <f>POWER(F10,2)/100</f>
-        <v>0.49406841000000001</v>
-      </c>
-      <c r="J10">
-        <f>(H10/D10)*100</f>
         <v>87.091205711263882</v>
       </c>
     </row>
@@ -2821,22 +2977,22 @@
         <v>2.6929999999999999E-2</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.80789999999999995</v>
       </c>
       <c r="F11">
         <v>8.4499999999999993</v>
       </c>
       <c r="G11">
+        <f t="shared" si="3"/>
+        <v>8.4499999999999992E-2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0.71402499999999991</v>
+      </c>
+      <c r="J11">
         <f t="shared" si="1"/>
-        <v>8.4499999999999992E-2</v>
-      </c>
-      <c r="H11">
-        <f>POWER(F11,2)/100</f>
-        <v>0.71402499999999991</v>
-      </c>
-      <c r="J11">
-        <f>(H11/D11)*100</f>
         <v>88.380368857531863</v>
       </c>
     </row>
@@ -2848,22 +3004,22 @@
         <v>3.637E-2</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.0911</v>
       </c>
       <c r="F12">
         <v>9.8699999999999992</v>
       </c>
       <c r="G12">
+        <f t="shared" si="3"/>
+        <v>9.8699999999999996E-2</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>0.97416899999999984</v>
+      </c>
+      <c r="J12">
         <f t="shared" si="1"/>
-        <v>9.8699999999999996E-2</v>
-      </c>
-      <c r="H12">
-        <f>POWER(F12,2)/100</f>
-        <v>0.97416899999999984</v>
-      </c>
-      <c r="J12">
-        <f>(H12/D12)*100</f>
         <v>89.283200439923007</v>
       </c>
     </row>
@@ -2875,22 +3031,22 @@
         <v>4.7300000000000002E-2</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.419</v>
       </c>
       <c r="F13">
         <v>11.284000000000001</v>
       </c>
       <c r="G13">
+        <f t="shared" si="3"/>
+        <v>0.11284000000000001</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>1.2732865600000001</v>
+      </c>
+      <c r="J13">
         <f t="shared" si="1"/>
-        <v>0.11284000000000001</v>
-      </c>
-      <c r="H13">
-        <f>POWER(F13,2)/100</f>
-        <v>1.2732865600000001</v>
-      </c>
-      <c r="J13">
-        <f>(H13/D13)*100</f>
         <v>89.731258632840024</v>
       </c>
     </row>
@@ -2902,22 +3058,22 @@
         <v>5.9499999999999997E-2</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.7849999999999999</v>
       </c>
       <c r="F14">
         <v>12.694000000000001</v>
       </c>
       <c r="G14">
+        <f t="shared" si="3"/>
+        <v>0.12694</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>1.6113763600000002</v>
+      </c>
+      <c r="J14">
         <f t="shared" si="1"/>
-        <v>0.12694</v>
-      </c>
-      <c r="H14">
-        <f>POWER(F14,2)/100</f>
-        <v>1.6113763600000002</v>
-      </c>
-      <c r="J14">
-        <f>(H14/D14)*100</f>
         <v>90.273185434173683</v>
       </c>
     </row>
@@ -2929,22 +3085,22 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.19</v>
       </c>
       <c r="F15">
         <v>14.090999999999999</v>
       </c>
       <c r="G15">
+        <f t="shared" si="3"/>
+        <v>0.14090999999999998</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>1.9855628099999998</v>
+      </c>
+      <c r="J15">
         <f t="shared" si="1"/>
-        <v>0.14090999999999998</v>
-      </c>
-      <c r="H15">
-        <f>POWER(F15,2)/100</f>
-        <v>1.9855628099999998</v>
-      </c>
-      <c r="J15">
-        <f>(H15/D15)*100</f>
         <v>90.664968493150681</v>
       </c>
     </row>
@@ -2956,22 +3112,22 @@
         <v>8.7900000000000006E-2</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.637</v>
       </c>
       <c r="F16">
         <v>15.48</v>
       </c>
       <c r="G16">
+        <f t="shared" si="3"/>
+        <v>0.15479999999999999</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>2.3963040000000002</v>
+      </c>
+      <c r="J16">
         <f t="shared" si="1"/>
-        <v>0.15479999999999999</v>
-      </c>
-      <c r="H16">
-        <f>POWER(F16,2)/100</f>
-        <v>2.3963040000000002</v>
-      </c>
-      <c r="J16">
-        <f>(H16/D16)*100</f>
         <v>90.872354948805466</v>
       </c>
     </row>
@@ -2983,22 +3139,22 @@
         <v>0.10390000000000001</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.117</v>
       </c>
       <c r="F17">
         <v>16.856000000000002</v>
       </c>
       <c r="G17">
+        <f t="shared" si="3"/>
+        <v>0.16856000000000002</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>2.8412473600000006</v>
+      </c>
+      <c r="J17">
         <f t="shared" si="1"/>
-        <v>0.16856000000000002</v>
-      </c>
-      <c r="H17">
-        <f>POWER(F17,2)/100</f>
-        <v>2.8412473600000006</v>
-      </c>
-      <c r="J17">
-        <f>(H17/D17)*100</f>
         <v>91.153267885787642</v>
       </c>
     </row>
@@ -3010,22 +3166,22 @@
         <v>0.12130000000000001</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.6390000000000002</v>
       </c>
       <c r="F18">
         <v>18.221</v>
       </c>
       <c r="G18">
+        <f t="shared" si="3"/>
+        <v>0.18221000000000001</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>3.3200484100000001</v>
+      </c>
+      <c r="J18">
         <f t="shared" si="1"/>
-        <v>0.18221000000000001</v>
-      </c>
-      <c r="H18">
-        <f>POWER(F18,2)/100</f>
-        <v>3.3200484100000001</v>
-      </c>
-      <c r="J18">
-        <f>(H18/D18)*100</f>
         <v>91.235185765320139</v>
       </c>
     </row>
@@ -3037,22 +3193,22 @@
         <v>0.13980000000000001</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.194</v>
       </c>
       <c r="F19">
         <v>19.568000000000001</v>
       </c>
       <c r="G19">
+        <f t="shared" si="3"/>
+        <v>0.19568000000000002</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>3.8290662400000008</v>
+      </c>
+      <c r="J19">
         <f t="shared" si="1"/>
-        <v>0.19568000000000002</v>
-      </c>
-      <c r="H19">
-        <f>POWER(F19,2)/100</f>
-        <v>3.8290662400000008</v>
-      </c>
-      <c r="J19">
-        <f>(H19/D19)*100</f>
         <v>91.298670481640471</v>
       </c>
     </row>
@@ -3064,22 +3220,22 @@
         <v>0.15970000000000001</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.7910000000000004</v>
       </c>
       <c r="F20">
         <v>20.905000000000001</v>
       </c>
       <c r="G20">
+        <f t="shared" si="3"/>
+        <v>0.20905000000000001</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>4.3701902500000003</v>
+      </c>
+      <c r="J20">
         <f t="shared" si="1"/>
-        <v>0.20905000000000001</v>
-      </c>
-      <c r="H20">
-        <f>POWER(F20,2)/100</f>
-        <v>4.3701902500000003</v>
-      </c>
-      <c r="J20">
-        <f>(H20/D20)*100</f>
         <v>91.21666144854936</v>
       </c>
     </row>
@@ -3091,22 +3247,22 @@
         <v>0.18079999999999999</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.4239999999999995</v>
       </c>
       <c r="F21">
         <v>22.227</v>
       </c>
       <c r="G21">
+        <f t="shared" si="3"/>
+        <v>0.22227</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>4.9403952900000005</v>
+      </c>
+      <c r="J21">
         <f t="shared" si="1"/>
-        <v>0.22227</v>
-      </c>
-      <c r="H21">
-        <f>POWER(F21,2)/100</f>
-        <v>4.9403952900000005</v>
-      </c>
-      <c r="J21">
-        <f>(H21/D21)*100</f>
         <v>91.083983960177008</v>
       </c>
     </row>
@@ -3118,22 +3274,22 @@
         <v>0.2029</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.0869999999999997</v>
       </c>
       <c r="F22">
         <v>23.529</v>
       </c>
       <c r="G22">
+        <f t="shared" si="3"/>
+        <v>0.23529</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>5.5361384099999995</v>
+      </c>
+      <c r="J22">
         <f t="shared" si="1"/>
-        <v>0.23529</v>
-      </c>
-      <c r="H22">
-        <f>POWER(F22,2)/100</f>
-        <v>5.5361384099999995</v>
-      </c>
-      <c r="J22">
-        <f>(H22/D22)*100</f>
         <v>90.95019566288812</v>
       </c>
     </row>
@@ -3145,22 +3301,22 @@
         <v>0.2263</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.7889999999999997</v>
       </c>
       <c r="F23">
         <v>24.814</v>
       </c>
       <c r="G23">
+        <f t="shared" si="3"/>
+        <v>0.24814</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>6.1573459599999998</v>
+      </c>
+      <c r="J23">
         <f t="shared" si="1"/>
-        <v>0.24814</v>
-      </c>
-      <c r="H23">
-        <f>POWER(F23,2)/100</f>
-        <v>6.1573459599999998</v>
-      </c>
-      <c r="J23">
-        <f>(H23/D23)*100</f>
         <v>90.695919281190157</v>
       </c>
     </row>
@@ -3172,22 +3328,22 @@
         <v>0.251</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.53</v>
       </c>
       <c r="F24">
         <v>26.082000000000001</v>
       </c>
       <c r="G24">
+        <f t="shared" si="3"/>
+        <v>0.26082</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>6.802707240000001</v>
+      </c>
+      <c r="J24">
         <f t="shared" si="1"/>
-        <v>0.26082</v>
-      </c>
-      <c r="H24">
-        <f>POWER(F24,2)/100</f>
-        <v>6.802707240000001</v>
-      </c>
-      <c r="J24">
-        <f>(H24/D24)*100</f>
         <v>90.341397609561767</v>
       </c>
     </row>

</xml_diff>